<commit_message>
Add snake movement and instantiate prey in random position
Add snake movment
Instantiate the prey in random position
Update backlog
</commit_message>
<xml_diff>
--- a/Product-backlog.xlsx
+++ b/Product-backlog.xlsx
@@ -977,8 +977,8 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="F10" s="34">
         <f>AVERAGEA(F12:K22)</f>
-        <v>0.2818181818181818</v>
+        <v>0.36153846153846153</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -1277,7 +1277,9 @@
       <c r="H18" s="33">
         <v>0.1</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="36">
+        <v>0.8</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
@@ -1293,6 +1295,9 @@
       </c>
       <c r="H19" s="33">
         <v>0.1</v>
+      </c>
+      <c r="I19" s="36">
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1411,6 +1416,9 @@
       <c r="F30" s="33">
         <v>0</v>
       </c>
+      <c r="I30" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
@@ -1440,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>4.3</v>
       </c>
@@ -1453,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>72</v>
       </c>
@@ -1463,8 +1471,11 @@
       <c r="F34" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I34" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>71</v>
       </c>
@@ -1475,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>4.4000000000000004</v>
       </c>
@@ -1488,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>4.5</v>
       </c>
@@ -1499,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
add snake eat prey
add snake eat prey
create new prey if snake eats one
show gameOver menu when loosing
</commit_message>
<xml_diff>
--- a/Product-backlog.xlsx
+++ b/Product-backlog.xlsx
@@ -977,8 +977,8 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="F10" s="34">
         <f>AVERAGEA(F12:K22)</f>
-        <v>0.36153846153846153</v>
+        <v>0.48124999999999996</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -1280,7 +1280,9 @@
       <c r="I18" s="36">
         <v>0.8</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="J18" s="36">
+        <v>1</v>
+      </c>
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1299,6 +1301,9 @@
       <c r="I19" s="36">
         <v>0.8</v>
       </c>
+      <c r="J19" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -1309,6 +1314,9 @@
       </c>
       <c r="F20" s="33">
         <v>0</v>
+      </c>
+      <c r="J20" s="36">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1361,6 +1369,9 @@
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
+      <c r="J25" s="36">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
@@ -1433,6 +1444,9 @@
       <c r="F31" s="33">
         <v>0</v>
       </c>
+      <c r="J31" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
@@ -1447,8 +1461,11 @@
       <c r="F32" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>4.3</v>
       </c>
@@ -1461,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>72</v>
       </c>
@@ -1475,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>71</v>
       </c>
@@ -1485,8 +1502,11 @@
       <c r="F35" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>4.4000000000000004</v>
       </c>
@@ -1499,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>4.5</v>
       </c>
@@ -1510,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>5</v>
       </c>

</xml_diff>